<commit_message>
US state encoding file update
</commit_message>
<xml_diff>
--- a/USA.xlsx
+++ b/USA.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barte\Documents\Data Science\Projekty\Projekt Future Collars\GitHub project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BDC486-E7BC-4473-A3D7-92ACACC81FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="150" windowWidth="22005" windowHeight="9240"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Geographic location" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="111">
   <si>
     <t>Alabama</t>
   </si>
@@ -24,9 +30,6 @@
     <t>AL</t>
   </si>
   <si>
-    <t>Alaska</t>
-  </si>
-  <si>
     <t>AK</t>
   </si>
   <si>
@@ -349,19 +352,30 @@
   </si>
   <si>
     <t>poverty_index_2019_(%)</t>
+  </si>
+  <si>
+    <t>Alasca</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Czcionka tekstu podstawowego"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -427,46 +441,66 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -513,7 +547,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -545,9 +579,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -579,6 +631,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -754,771 +824,781 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="15.75" customWidth="1"/>
-    <col min="2" max="2" width="15.625" customWidth="1"/>
+    <col min="1" max="1" width="15.69921875" customWidth="1"/>
+    <col min="2" max="2" width="15.59765625" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
     <col min="4" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="33.75" customWidth="1"/>
-    <col min="9" max="9" width="15.75" customWidth="1"/>
+    <col min="5" max="5" width="33.69921875" customWidth="1"/>
+    <col min="9" max="9" width="15.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
+    <row r="1" spans="1:5" ht="14.4">
       <c r="A1" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="15">
+    <row r="2" spans="1:5" ht="14.4">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" ht="15">
+    <row r="3" spans="1:5" ht="14.4">
       <c r="A3" s="1" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" ht="15">
+    <row r="4" spans="1:5" ht="14.4">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" ht="15">
+    <row r="5" spans="1:5" ht="14.4">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" ht="15">
+    <row r="6" spans="1:5" ht="14.4">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="15">
+    <row r="7" spans="1:5" ht="14.4">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="15">
+    <row r="8" spans="1:5" ht="14.4">
       <c r="A8" s="1" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" ht="15">
+    <row r="9" spans="1:5" ht="14.4">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="15">
+    <row r="10" spans="1:5" ht="14.4">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="15">
+    <row r="11" spans="1:5" ht="14.4">
       <c r="A11" s="1" t="s">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="15">
+    <row r="12" spans="1:5" ht="14.4">
       <c r="A12" s="1" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="15">
+    <row r="13" spans="1:5" ht="14.4">
       <c r="A13" s="1" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" ht="15">
+    <row r="14" spans="1:5" ht="14.4">
       <c r="A14" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" ht="15">
+    <row r="15" spans="1:5" ht="14.4">
       <c r="A15" s="1" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" ht="15">
+    <row r="16" spans="1:5" ht="14.4">
       <c r="A16" s="1" t="s">
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>97</v>
+        <v>26</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="15">
+    <row r="17" spans="1:5" ht="14.4">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="15">
+    <row r="18" spans="1:5" ht="14.4">
       <c r="A18" s="1" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="15">
+    <row r="19" spans="1:5" ht="14.4">
       <c r="A19" s="1" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" ht="15">
+    <row r="20" spans="1:5" ht="14.4">
       <c r="A20" s="1" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="15">
+    <row r="21" spans="1:5" ht="14.4">
       <c r="A21" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="15">
+    <row r="22" spans="1:5" ht="14.4">
       <c r="A22" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" ht="15">
+    <row r="23" spans="1:5" ht="14.4">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" ht="15">
-      <c r="A24" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>53</v>
+    <row r="24" spans="1:5" ht="15" thickBot="1">
+      <c r="A24" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A25" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>53</v>
+    <row r="25" spans="1:5" ht="15" thickTop="1">
+      <c r="A25" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>101</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" ht="15.75" thickTop="1">
+    <row r="26" spans="1:5" ht="14.4">
       <c r="A26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>93</v>
-      </c>
       <c r="C26" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" ht="15">
+    <row r="27" spans="1:5" ht="14.4">
       <c r="A27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>67</v>
-      </c>
       <c r="C27" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5" ht="15">
+    <row r="28" spans="1:5" ht="14.4">
       <c r="A28" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" ht="15">
+    <row r="29" spans="1:5" ht="14.4">
       <c r="A29" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>99</v>
-      </c>
       <c r="C29" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5" ht="15">
+    <row r="30" spans="1:5" ht="14.4">
       <c r="A30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>11</v>
-      </c>
       <c r="C30" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" ht="15">
+    <row r="31" spans="1:5" ht="14.4">
       <c r="A31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B31" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="C31" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" ht="15">
+    <row r="32" spans="1:5" ht="14.4">
       <c r="A32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>31</v>
-      </c>
       <c r="C32" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="1:5" ht="15">
+    <row r="33" spans="1:5" ht="14.4">
       <c r="A33" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>87</v>
-      </c>
       <c r="C33" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:5" ht="15">
+    <row r="34" spans="1:5" ht="14.4">
       <c r="A34" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>73</v>
-      </c>
       <c r="C34" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:5" ht="15">
+    <row r="35" spans="1:5" ht="14.4">
       <c r="A35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="7" t="s">
-        <v>51</v>
-      </c>
       <c r="C35" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A36" s="12" t="s">
+    <row r="36" spans="1:5" ht="14.4">
+      <c r="A36" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>102</v>
+      <c r="C36" s="16" t="s">
+        <v>101</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="1:5" ht="15.75" thickTop="1">
-      <c r="A37" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>100</v>
+    <row r="37" spans="1:5" ht="15" thickBot="1">
+      <c r="A37" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>101</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="5"/>
     </row>
-    <row r="38" spans="1:5" ht="15">
+    <row r="38" spans="1:5" ht="15" thickTop="1">
       <c r="A38" s="1" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="5"/>
     </row>
-    <row r="39" spans="1:5" ht="15">
+    <row r="39" spans="1:5" ht="14.4">
       <c r="A39" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="5"/>
     </row>
-    <row r="40" spans="1:5" ht="15">
+    <row r="40" spans="1:5" ht="14.4">
       <c r="A40" s="1" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="5"/>
     </row>
-    <row r="41" spans="1:5" ht="15">
+    <row r="41" spans="1:5" ht="14.4">
       <c r="A41" s="1" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="5"/>
     </row>
-    <row r="42" spans="1:5" ht="15">
+    <row r="42" spans="1:5" ht="14.4">
       <c r="A42" s="1" t="s">
-        <v>78</v>
+        <v>33</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="5"/>
     </row>
-    <row r="43" spans="1:5" ht="15">
+    <row r="43" spans="1:5" ht="14.4">
       <c r="A43" s="1" t="s">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>1</v>
+        <v>78</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="5"/>
     </row>
-    <row r="44" spans="1:5" ht="15">
+    <row r="44" spans="1:5" ht="14.4">
       <c r="A44" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="5"/>
     </row>
-    <row r="45" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A45" s="12" t="s">
+    <row r="45" spans="1:5" ht="14.4">
+      <c r="A45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="5"/>
+    </row>
+    <row r="46" spans="1:5" ht="15" thickBot="1">
+      <c r="A46" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B45" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C45" s="13" t="s">
+      <c r="C46" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47" spans="1:5" ht="15" thickTop="1">
+      <c r="A47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="D45" s="2"/>
-      <c r="E45" s="6"/>
-    </row>
-    <row r="46" spans="1:5" ht="15.75" thickTop="1">
-      <c r="A46" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D46" s="2"/>
-      <c r="E46" s="5"/>
-    </row>
-    <row r="47" spans="1:5" ht="15">
-      <c r="A47" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="5"/>
     </row>
-    <row r="48" spans="1:5" ht="15">
+    <row r="48" spans="1:5" ht="14.4">
       <c r="A48" s="1" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="5"/>
     </row>
-    <row r="49" spans="1:10" ht="15">
+    <row r="49" spans="1:10" ht="14.4">
       <c r="A49" s="1" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="5"/>
     </row>
-    <row r="50" spans="1:10" ht="15">
+    <row r="50" spans="1:10" ht="14.4">
       <c r="A50" s="1" t="s">
-        <v>70</v>
+        <v>3</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="5"/>
     </row>
-    <row r="51" spans="1:10" ht="15">
+    <row r="51" spans="1:10" ht="14.4">
       <c r="A51" s="1" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="5"/>
     </row>
-    <row r="52" spans="1:10" ht="15">
+    <row r="52" spans="1:10" ht="14.4">
       <c r="A52" s="1" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="5"/>
     </row>
-    <row r="57" spans="1:10">
-      <c r="J57" s="4"/>
+    <row r="53" spans="1:10" ht="14.4">
+      <c r="A53" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" s="5"/>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="J58" s="4"/>
     </row>
   </sheetData>
-  <sortState ref="A2:E51">
-    <sortCondition ref="C2"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:I53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="7.25" customWidth="1"/>
-    <col min="2" max="2" width="15.875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="7.19921875" customWidth="1"/>
+    <col min="2" max="2" width="15.8984375" style="9" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="7" max="7" width="20.5" customWidth="1"/>
-    <col min="8" max="8" width="43.25" style="9" customWidth="1"/>
+    <col min="8" max="8" width="43.19921875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="15.75" customHeight="1">
       <c r="B2" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="G2" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" ht="15">
+    </row>
+    <row r="3" spans="2:8" ht="14.4">
       <c r="B3" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="8">
         <v>42.75</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H3" s="7">
         <v>7.3</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="15">
+    <row r="4" spans="2:8" ht="14.4">
       <c r="B4" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="8">
         <v>48.314</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H4" s="7">
         <v>8.9</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="15">
+    <row r="5" spans="2:8" ht="14.4">
       <c r="B5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1526,592 +1606,592 @@
         <v>49.305</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H5" s="7">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="15">
+    <row r="6" spans="2:8" ht="14.4">
       <c r="B6" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="8">
         <v>49.335999999999999</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H6" s="7">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="15">
+    <row r="7" spans="2:8" ht="14.4">
       <c r="B7" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C7" s="8">
         <v>49.463999999999999</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H7" s="7">
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="15">
+    <row r="8" spans="2:8" ht="14.4">
       <c r="B8" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" s="8">
         <v>52.23</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H8" s="7">
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="15">
+    <row r="9" spans="2:8" ht="14.4">
       <c r="B9" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="8">
         <v>52.290999999999997</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H9" s="7">
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="15">
+    <row r="10" spans="2:8" ht="14.4">
       <c r="B10" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" s="8">
         <v>52.912999999999997</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H10" s="7">
         <v>9.4</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="15">
+    <row r="11" spans="2:8" ht="14.4">
       <c r="B11" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="8">
         <v>53.034999999999997</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H11" s="7">
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="15">
+    <row r="12" spans="2:8" ht="14.4">
       <c r="B12" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="8">
         <v>53.448</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H12" s="7">
         <v>9.9</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="15">
+    <row r="13" spans="2:8" ht="14.4">
       <c r="B13" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="8">
         <v>55.375</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H13" s="7">
         <v>9.9</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="15">
+    <row r="14" spans="2:8" ht="14.4">
       <c r="B14" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="8">
         <v>55.558</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H14" s="7">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="15">
+    <row r="15" spans="2:8" ht="14.4">
       <c r="B15" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" s="8">
         <v>56.273000000000003</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H15" s="7">
         <v>10.1</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="15">
+    <row r="16" spans="2:8" ht="14.4">
       <c r="B16" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="8">
         <v>56.325000000000003</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H16" s="7">
         <v>10.1</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="15">
+    <row r="17" spans="2:9" ht="14.4">
       <c r="B17" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" s="8">
         <v>56.457999999999998</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H17" s="7">
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="15">
+    <row r="18" spans="2:9" ht="14.4">
       <c r="B18" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C18" s="8">
         <v>56.692999999999998</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H18" s="7">
         <v>10.4</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="15">
+    <row r="19" spans="2:9" ht="14.4">
       <c r="B19" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" s="8">
         <v>59.302</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H19" s="7">
         <v>10.6</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="15">
+    <row r="20" spans="2:9" ht="14.4">
       <c r="B20" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C20" s="8">
         <v>59.595999999999997</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H20" s="7">
         <v>10.8</v>
       </c>
       <c r="I20" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" ht="15">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="14.4">
       <c r="B21" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C21" s="8">
         <v>60.354999999999997</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H21" s="7">
         <v>10.9</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="15">
+    <row r="22" spans="2:9" ht="14.4">
       <c r="B22" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="8">
         <v>61.101999999999997</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H22" s="7">
         <v>11.2</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="15">
+    <row r="23" spans="2:9" ht="14.4">
       <c r="B23" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" s="8">
         <v>62.14</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H23" s="7">
         <v>11.2</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="15">
+    <row r="24" spans="2:9" ht="14.4">
       <c r="B24" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C24" s="8">
         <v>62.505000000000003</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H24" s="7">
         <v>11.3</v>
       </c>
     </row>
-    <row r="25" spans="2:9" ht="15">
+    <row r="25" spans="2:9" ht="14.4">
       <c r="B25" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C25" s="8">
         <v>62.587000000000003</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H25" s="7">
         <v>11.4</v>
       </c>
     </row>
-    <row r="26" spans="2:9" ht="15">
+    <row r="26" spans="2:9" ht="14.4">
       <c r="B26" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C26" s="8">
         <v>63.23</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H26" s="7">
         <v>11.4</v>
       </c>
     </row>
-    <row r="27" spans="2:9" ht="15">
+    <row r="27" spans="2:9" ht="14.4">
       <c r="B27" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C27" s="8">
         <v>63.585000000000001</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H27" s="7">
         <v>11.5</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="15">
+    <row r="28" spans="2:9" ht="14.4">
       <c r="B28" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" s="8">
         <v>63.67</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H28" s="7">
         <v>11.8</v>
       </c>
     </row>
-    <row r="29" spans="2:9" ht="15">
+    <row r="29" spans="2:9" ht="14.4">
       <c r="B29" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C29" s="8">
         <v>64.084000000000003</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H29" s="7">
         <v>11.9</v>
       </c>
     </row>
-    <row r="30" spans="2:9" ht="15">
+    <row r="30" spans="2:9" ht="14.4">
       <c r="B30" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C30" s="8">
         <v>65.162000000000006</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H30" s="7">
         <v>11.9</v>
       </c>
     </row>
-    <row r="31" spans="2:9" ht="15">
+    <row r="31" spans="2:9" ht="14.4">
       <c r="B31" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C31" s="8">
         <v>65.543999999999997</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H31" s="7">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="2:9" ht="15">
+    <row r="32" spans="2:9" ht="14.4">
       <c r="B32" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32" s="8">
         <v>66.936999999999998</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H32" s="7">
         <v>12.5</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="15">
+    <row r="33" spans="2:8" ht="14.4">
       <c r="B33" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C33" s="8">
         <v>67.84</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H33" s="7">
         <v>12.6</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="15">
+    <row r="34" spans="2:8" ht="14.4">
       <c r="B34" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C34" s="8">
         <v>67.951999999999998</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H34" s="7">
         <v>12.7</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="15">
+    <row r="35" spans="2:8" ht="14.4">
       <c r="B35" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C35" s="8">
         <v>68.718999999999994</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H35" s="7">
         <v>12.9</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="15">
+    <row r="36" spans="2:8" ht="14.4">
       <c r="B36" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C36" s="8">
         <v>69.183000000000007</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H36" s="7">
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="15">
+    <row r="37" spans="2:8" ht="14.4">
       <c r="B37" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C37" s="8">
         <v>70.465999999999994</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H37" s="7">
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="15">
+    <row r="38" spans="2:8" ht="14.4">
       <c r="B38" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C38" s="8">
         <v>72.77</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H38" s="7">
         <v>13.1</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="15">
+    <row r="39" spans="2:8" ht="14.4">
       <c r="B39" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C39" s="8">
         <v>73.218000000000004</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H39" s="7">
         <v>13.3</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="15">
+    <row r="40" spans="2:8" ht="14.4">
       <c r="B40" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C40" s="8">
         <v>73.245000000000005</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H40" s="7">
         <v>13.5</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="15">
+    <row r="41" spans="2:8" ht="14.4">
       <c r="B41" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C41" s="8">
         <v>73.352000000000004</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H41" s="7">
         <v>13.5</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="15">
+    <row r="42" spans="2:8" ht="14.4">
       <c r="B42" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C42" s="8">
         <v>74.111999999999995</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H42" s="7">
         <v>13.6</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="15">
+    <row r="43" spans="2:8" ht="14.4">
       <c r="B43" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C43" s="8">
         <v>75.462000000000003</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H43" s="7">
         <v>13.6</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="15">
+    <row r="44" spans="2:8" ht="14.4">
       <c r="B44" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C44" s="8">
         <v>75.706999999999994</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H44" s="7">
         <v>13.8</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="15">
+    <row r="45" spans="2:8" ht="14.4">
       <c r="B45" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C45" s="8">
         <v>78.132999999999996</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H45" s="7">
         <v>13.9</v>
       </c>
     </row>
-    <row r="46" spans="2:8" ht="15">
+    <row r="46" spans="2:8" ht="14.4">
       <c r="B46" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C46" s="8">
         <v>80.584999999999994</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H46" s="7">
         <v>15.2</v>
       </c>
     </row>
-    <row r="47" spans="2:8" ht="15">
+    <row r="47" spans="2:8" ht="14.4">
       <c r="B47" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C47" s="8">
         <v>83.147000000000006</v>
@@ -2123,92 +2203,92 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="15">
+    <row r="48" spans="2:8" ht="14.4">
       <c r="B48" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C48" s="8">
         <v>85.46</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H48" s="7">
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="2:8" ht="15">
+    <row r="49" spans="2:8" ht="14.4">
       <c r="B49" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C49" s="8">
         <v>85.765000000000001</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H49" s="7">
         <v>16.2</v>
       </c>
     </row>
-    <row r="50" spans="2:8" ht="15">
+    <row r="50" spans="2:8" ht="14.4">
       <c r="B50" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C50" s="8">
         <v>86.975999999999999</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H50" s="7">
         <v>16.3</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="15">
+    <row r="51" spans="2:8" ht="14.4">
       <c r="B51" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C51" s="8">
         <v>91.233000000000004</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H51" s="7">
         <v>18.2</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="15">
+    <row r="52" spans="2:8" ht="14.4">
       <c r="B52" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C52" s="8">
         <v>95.447000000000003</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H52" s="7">
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="2:8" ht="15">
+    <row r="53" spans="2:8" ht="14.4">
       <c r="B53" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C53" s="8">
         <v>229.80199999999999</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H53" s="8">
         <v>20.3</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="G3:I53">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G3:I53">
     <sortCondition ref="H3:H53"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2217,12 +2297,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>